<commit_message>
sps: Add perf test results
Scope: SafeguardSessions/PerformanceTesting/Results.xlsx

Add perf test results of the test round started on 2023.08.28. The
`Template` spreadsheet is removed since with the new test round's
spreadsheet it became an unnecessary duplication. We can copy the
previous test round's spreadsheet when we start a new perf test.

References: azure #422230
</commit_message>
<xml_diff>
--- a/SafeguardSessions/PerformanceTesting/Results.xlsx
+++ b/SafeguardSessions/PerformanceTesting/Results.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddavid\Repos\SafeguardPowerBI\SafeguardSessions\assets\performance_testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddavid\Repos\SafeguardPowerBI\SafeguardSessions\PerformanceTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E12C232-D985-4E97-BCA0-51F3ECC956A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB61D66-7062-492C-AF04-75C293D916F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28350" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28350" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="2023.08.28" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -60,7 +60,7 @@
 (release version, tag or commit SHA)</t>
   </si>
   <si>
-    <t>6e4393b583</t>
+    <t>7.4.0.alpha1</t>
   </si>
   <si>
     <t>Auth succeeded SSH sessions</t>
@@ -82,9 +82,6 @@
 (release version, tag or commit SHA)</t>
   </si>
   <si>
-    <t>v1.1.1pre2+sps7.4.0</t>
-  </si>
-  <si>
     <t>Sessions in total</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
     <t>Measurement</t>
   </si>
   <si>
+    <t>Baseline SPS performance</t>
+  </si>
+  <si>
     <t>Basic scenario (initial import)</t>
   </si>
   <si>
@@ -121,10 +121,42 @@
     <t>Worst-case scenario (refresh)</t>
   </si>
   <si>
-    <t>Start time</t>
-  </si>
-  <si>
-    <t>End time</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Start time (UTC) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC65911"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">End time (UTC) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC65911"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
   </si>
   <si>
     <t>Duration</t>
@@ -175,10 +207,32 @@
     <t>Pipeline error count</t>
   </si>
   <si>
-    <t>Baseline SPS performance</t>
-  </si>
-  <si>
-    <t>N/A</t>
+    <t>307ade9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC65911"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For Baseline SPS performance start-, end times refer to when the SPS performance test ran.
+For scenarios, they refer to the start and end time of the data import into Power BI.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -188,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +283,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC65911"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC65911"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFC65911"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -256,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -386,30 +486,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -432,94 +514,91 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -836,11 +915,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9716B4-9E5F-4437-941A-9D9481CCBD0E}">
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +951,7 @@
       <c r="L1" s="21"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="23"/>
@@ -903,20 +982,20 @@
         <v>6</v>
       </c>
       <c r="E3" s="27"/>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="36">
+      <c r="H3" s="31"/>
+      <c r="I3" s="34">
         <v>1500000</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="22"/>
+      <c r="K3" s="29"/>
       <c r="L3" s="5">
         <v>750000</v>
       </c>
@@ -927,14 +1006,14 @@
       <c r="C4" s="26"/>
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="22" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="22"/>
+      <c r="K4" s="29"/>
       <c r="L4" s="5">
         <v>750000</v>
       </c>
@@ -943,43 +1022,43 @@
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="22" t="s">
+      <c r="E5" s="38"/>
+      <c r="F5" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="4">
         <v>1500000</v>
       </c>
-      <c r="J5" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="22"/>
+      <c r="J5" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="29"/>
       <c r="L5" s="5">
         <v>1500000</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="22"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="29"/>
       <c r="G6" s="6"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -989,12 +1068,12 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1007,14 +1086,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1024,680 +1103,695 @@
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
+      <c r="A9" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18" t="s">
+      <c r="B10" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18" t="s">
+      <c r="G10" s="37"/>
+      <c r="H10" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18" t="s">
+      <c r="I10" s="37"/>
+      <c r="J10" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="37"/>
       <c r="L10" s="14"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>46</v>
+      <c r="B11" s="41">
+        <v>45166.648854166669</v>
       </c>
       <c r="C11" s="41"/>
-      <c r="D11" s="39">
-        <v>45159.24355324074</v>
-      </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39">
-        <v>45159.24355324074</v>
-      </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39">
-        <v>45159.24355324074</v>
-      </c>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39">
-        <v>45159.24355324074</v>
-      </c>
-      <c r="K11" s="39"/>
+      <c r="D11" s="41">
+        <v>45190.437268518515</v>
+      </c>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41">
+        <v>45190.609722222223</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41">
+        <v>45194.51458333333</v>
+      </c>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41">
+        <v>45194.806250000001</v>
+      </c>
+      <c r="K11" s="41"/>
       <c r="L11" s="14"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="39">
-        <v>45159.243877314817</v>
-      </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39">
-        <v>45159.243877314817</v>
-      </c>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39">
-        <v>45159.243877314817</v>
-      </c>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39">
-        <v>45159.243877314817</v>
-      </c>
-      <c r="K12" s="39"/>
+      <c r="B12" s="41">
+        <v>45166.782754629632</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41">
+        <v>45190.515972222223</v>
+      </c>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41">
+        <v>45190.69027777778</v>
+      </c>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41">
+        <v>45194.589583333334</v>
+      </c>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41">
+        <v>45194.884027777778</v>
+      </c>
+      <c r="K12" s="41"/>
       <c r="L12" s="14"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="38">
+      <c r="B13" s="39">
+        <f>B12-B11</f>
+        <v>0.13390046296262881</v>
+      </c>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39">
         <f>D12-D11</f>
-        <v>3.2407407707069069E-4</v>
-      </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38">
+        <v>7.8703703708015382E-2</v>
+      </c>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39">
         <f t="shared" ref="F13" si="0">F12-F11</f>
-        <v>3.2407407707069069E-4</v>
-      </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38">
-        <f t="shared" ref="H13" si="1">H12-H11</f>
-        <v>3.2407407707069069E-4</v>
-      </c>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38">
-        <f t="shared" ref="J13" si="2">J12-J11</f>
-        <v>3.2407407707069069E-4</v>
-      </c>
-      <c r="K13" s="38"/>
+        <v>8.0555555556202307E-2</v>
+      </c>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39">
+        <f>H12-H11</f>
+        <v>7.5000000004365575E-2</v>
+      </c>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39">
+        <f>J12-J11</f>
+        <v>7.7777777776645962E-2</v>
+      </c>
+      <c r="K13" s="39"/>
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="17">
-        <v>42.8</v>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17">
-        <v>42.8</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17">
-        <v>42.8</v>
-      </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17">
-        <v>42.8</v>
-      </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17">
-        <v>42.8</v>
-      </c>
-      <c r="K14" s="17"/>
+      <c r="B14" s="40">
+        <v>21.5</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40">
+        <v>22.7</v>
+      </c>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40">
+        <v>22.9</v>
+      </c>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40">
+        <v>22.7</v>
+      </c>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40">
+        <v>22.3</v>
+      </c>
+      <c r="K14" s="40"/>
       <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="17">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17">
-        <v>81.400000000000006</v>
-      </c>
-      <c r="K15" s="17"/>
+      <c r="B15" s="40">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40">
+        <v>32.9</v>
+      </c>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40">
+        <v>33</v>
+      </c>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="K15" s="40"/>
       <c r="L15" s="14"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="17">
-        <v>26.5</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17">
-        <v>26.5</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17">
-        <v>26.5</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17">
-        <v>26.5</v>
-      </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17">
-        <v>26.5</v>
-      </c>
-      <c r="K16" s="17"/>
+      <c r="B16" s="40">
+        <v>26.2</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40">
+        <v>35.9</v>
+      </c>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40">
+        <v>36.6</v>
+      </c>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40">
+        <v>33.1</v>
+      </c>
+      <c r="K16" s="40"/>
       <c r="L16" s="14"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="17">
-        <v>27.4</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17">
-        <v>27.4</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17">
-        <v>27.4</v>
-      </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17">
-        <v>27.4</v>
-      </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17">
-        <v>27.4</v>
-      </c>
-      <c r="K17" s="17"/>
+      <c r="B17" s="40">
+        <v>27.7</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40">
+        <v>36.1</v>
+      </c>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40">
+        <v>36.5</v>
+      </c>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40">
+        <v>36.9</v>
+      </c>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="K17" s="40"/>
       <c r="L17" s="14"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
       <c r="L18" s="14"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="17">
-        <v>3.05</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17">
-        <v>3.05</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17">
-        <v>3.05</v>
-      </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17">
-        <v>3.05</v>
-      </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17">
-        <v>3.05</v>
-      </c>
-      <c r="K19" s="17"/>
+      <c r="B19" s="40">
+        <v>1.3</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40">
+        <v>0.77</v>
+      </c>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40">
+        <v>0.71299999999999997</v>
+      </c>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="K19" s="40"/>
       <c r="L19" s="14"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="17">
-        <v>1.02</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17">
-        <v>1.02</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17">
-        <v>1.02</v>
-      </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17">
-        <v>1.02</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17">
-        <v>1.02</v>
-      </c>
-      <c r="K20" s="17"/>
+      <c r="B20" s="40">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="K20" s="40"/>
       <c r="L20" s="14"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
       <c r="L21" s="14"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="17">
-        <v>5.27</v>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17">
-        <v>5.27</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17">
-        <v>5.27</v>
-      </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17">
-        <v>5.27</v>
-      </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17">
-        <v>5.27</v>
-      </c>
-      <c r="K22" s="17"/>
+      <c r="B22" s="40">
+        <v>2.14</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40">
+        <v>1.34</v>
+      </c>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40">
+        <v>1.47</v>
+      </c>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40">
+        <v>1.24</v>
+      </c>
+      <c r="K22" s="40"/>
       <c r="L22" s="14"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="17">
-        <v>1.61</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17">
-        <v>1.61</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17">
-        <v>1.61</v>
-      </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17">
-        <v>1.61</v>
-      </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17">
-        <v>1.61</v>
-      </c>
-      <c r="K23" s="17"/>
+      <c r="B23" s="40">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40">
+        <v>1.29</v>
+      </c>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="K23" s="40"/>
       <c r="L23" s="14"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
       <c r="L24" s="14"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="17">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="K25" s="17"/>
+      <c r="B25" s="40">
+        <v>28.6</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40">
+        <v>55.8</v>
+      </c>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40">
+        <v>57</v>
+      </c>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40">
+        <v>51.8</v>
+      </c>
+      <c r="K25" s="40"/>
       <c r="L25" s="14"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="17">
-        <v>0</v>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17">
-        <v>0</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17">
-        <v>0</v>
-      </c>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17">
-        <v>0</v>
-      </c>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17">
-        <v>0</v>
-      </c>
-      <c r="K26" s="17"/>
+      <c r="B26" s="40">
+        <v>5.2</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40">
+        <v>5.44</v>
+      </c>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40">
+        <v>5.25</v>
+      </c>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40">
+        <v>1.9</v>
+      </c>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40">
+        <v>3.56</v>
+      </c>
+      <c r="K26" s="40"/>
       <c r="L26" s="14"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="17">
-        <v>33.1</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17">
-        <v>33.1</v>
-      </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17">
-        <v>33.1</v>
-      </c>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17">
-        <v>33.1</v>
-      </c>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17">
-        <v>33.1</v>
-      </c>
-      <c r="K27" s="17"/>
+      <c r="B27" s="40">
+        <v>57.2</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40">
+        <v>53.5</v>
+      </c>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40">
+        <v>52.9</v>
+      </c>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40">
+        <v>55.5</v>
+      </c>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40">
+        <v>48.9</v>
+      </c>
+      <c r="K27" s="40"/>
       <c r="L27" s="14"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="17">
-        <v>0.115</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17">
-        <v>0.115</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17">
-        <v>0.115</v>
-      </c>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17">
-        <v>0.115</v>
-      </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17">
-        <v>0.115</v>
-      </c>
-      <c r="K28" s="17"/>
+      <c r="B28" s="40">
+        <v>0.222</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40">
+        <v>0.214</v>
+      </c>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40">
+        <v>0.21</v>
+      </c>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40">
+        <v>0.18</v>
+      </c>
+      <c r="K28" s="40"/>
       <c r="L28" s="14"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="17">
-        <v>45.1</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17">
-        <v>45.1</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17">
-        <v>45.1</v>
-      </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17">
-        <v>45.1</v>
-      </c>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17">
-        <v>45.1</v>
-      </c>
-      <c r="K29" s="17"/>
+      <c r="B29" s="40">
+        <v>893</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40">
+        <v>245</v>
+      </c>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40">
+        <v>233</v>
+      </c>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40">
+        <v>676</v>
+      </c>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40">
+        <v>83.8</v>
+      </c>
+      <c r="K29" s="40"/>
       <c r="L29" s="14"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="16">
+      <c r="B30" s="44">
         <v>0</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16">
+      <c r="C30" s="44"/>
+      <c r="D30" s="44">
         <v>0</v>
       </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16">
+      <c r="E30" s="44"/>
+      <c r="F30" s="44">
         <v>0</v>
       </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16">
+      <c r="G30" s="44"/>
+      <c r="H30" s="44">
         <v>0</v>
       </c>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16">
+      <c r="I30" s="44"/>
+      <c r="J30" s="44">
         <v>0</v>
       </c>
-      <c r="K30" s="16"/>
+      <c r="K30" s="44"/>
       <c r="L30" s="15"/>
     </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="43"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+    </row>
   </sheetData>
-  <mergeCells count="124">
+  <mergeCells count="127">
+    <mergeCell ref="A31:E32"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="A9:L9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="A3:C4"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:H4"/>
     <mergeCell ref="I3:I4"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="A3:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="D5:E6"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B11:C13"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A3:C4" r:id="rId1" location="TOPIC-2021538" display="Help: Hardware specifications table" xr:uid="{7A8CD902-7717-4D9E-8E23-2C949694525A}"/>
+    <hyperlink ref="A3:C4" r:id="rId1" location="TOPIC-2021538" display="Help: Hardware specifications table" xr:uid="{7E3FA09E-A45D-4726-BC9D-7371A9B19F6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E9ABA3205C1457439534CE3DAF5F0726" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7719b9839725a7e9b53ef4babdd16a67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="22b0a55a-e510-419c-a4ee-932afbf3032e" xmlns:ns3="41f7933d-0400-4b1c-a588-00c817e14f4e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ea1a19a9021b43459927f99c6d9ce02" ns2:_="" ns3:_="">
     <xsd:import namespace="22b0a55a-e510-419c-a4ee-932afbf3032e"/>
@@ -1932,6 +2026,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1944,14 +2047,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E6C1AD-222C-47C7-89E9-95E0A1337C9A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDCD546B-5D53-432D-A84D-DB63C0EAF4AB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1970,6 +2065,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E6C1AD-222C-47C7-89E9-95E0A1337C9A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02CC1CB7-773C-43BC-9FE1-E1D2690FF897}">
   <ds:schemaRefs>

</xml_diff>